<commit_message>
updateLAOs results and tests
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [target].xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [target].xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/LAOs/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_86F279D926C198CE8A160BD92BDEC1CF751C1DD1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B923F291-EF47-4C68-BA14-BF35F5A11DB7}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capital and operating costs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" iterateDelta="9.9999999999994451E-4"/>
 </workbook>
 </file>
 
@@ -106,6 +112,18 @@
     <t>Total variable operating cost</t>
   </si>
   <si>
+    <t>DAP</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>Wastewater</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
     <t>Process water</t>
   </si>
   <si>
@@ -113,18 +131,6 @@
   </si>
   <si>
     <t>CSL</t>
-  </si>
-  <si>
-    <t>DAP</t>
-  </si>
-  <si>
-    <t>Salt</t>
-  </si>
-  <si>
-    <t>Wastewater</t>
-  </si>
-  <si>
-    <t>Glucose</t>
   </si>
   <si>
     <t>Natural gas</t>
@@ -154,8 +160,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -218,6 +227,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -264,7 +281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,9 +313,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,6 +365,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,14 +558,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,10 +589,10 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>65.5599881781126</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>65.787766180879586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -539,10 +600,10 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>32.40252089704887</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>32.116801970507218</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,10 +611,10 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>2.622399527124504</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>2.6315106472351841</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -561,10 +622,10 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>5.900398936030134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>5.9208989562791627</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -572,10 +633,10 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>2.950199468015067</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>2.9604494781395809</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -583,10 +644,10 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>109.4355070063312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>109.4174272330407</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -594,10 +655,10 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>10.94355070063312</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>10.94174272330407</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -605,10 +666,10 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>10.94355070063312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>10.94174272330407</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -616,10 +677,10 @@
         <v>22</v>
       </c>
       <c r="C11">
-        <v>21.88710140126624</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>21.883485446608152</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -627,10 +688,10 @@
         <v>23</v>
       </c>
       <c r="C12">
-        <v>32.83065210189935</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
+        <v>32.825228169912222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -638,10 +699,10 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>10.94355070063312</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>10.94174272330407</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -649,10 +710,10 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>87.54840560506497</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>87.533941786432621</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -660,10 +721,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>196.9839126113961</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>196.95136901947339</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -671,10 +732,10 @@
         <v>24</v>
       </c>
       <c r="C16">
-        <v>9.849195630569808</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>9.8475684509736681</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -682,10 +743,10 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>206.8331082419659</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>206.79893747044699</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
@@ -693,118 +754,118 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21">
-        <v>0.320236305</v>
+        <v>895.39159499999994</v>
       </c>
       <c r="D21">
-        <v>0.9953431044926841</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1"/>
+        <v>1.1811074895224249</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C22">
-        <v>775.6431749999999</v>
+        <v>136.07775000000001</v>
       </c>
       <c r="D22">
-        <v>-0.0007582707483223077</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1"/>
+        <v>4.2304986641846387</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C23">
-        <v>51.528108</v>
+        <v>-1.9630611699040379</v>
       </c>
       <c r="D23">
-        <v>0.5665068916007165</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1"/>
+        <v>-6.2658539245062812</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C24">
-        <v>895.3915949999999</v>
+        <v>244.03276500000001</v>
       </c>
       <c r="D24">
-        <v>1.181100356367396</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1"/>
+        <v>146.92179801857401</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>136.07775</v>
+        <v>0.320236305</v>
       </c>
       <c r="D25">
-        <v>4.230473398507108</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>0.99534905024449527</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C26">
-        <v>-1.963060763773765</v>
+        <v>878.15507999999988</v>
       </c>
       <c r="D26">
-        <v>-6.265815354911118</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>27</v>
-      </c>
+        <v>2.4024701315892168E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C27">
-        <v>235.999641825</v>
+        <v>51.528108000000003</v>
       </c>
       <c r="D27">
-        <v>142.0853945930931</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1"/>
+        <v>0.56651201273216611</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C28">
-        <v>197.76633</v>
+        <v>197.76633000000001</v>
       </c>
       <c r="D28">
-        <v>3.954641812231309</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>3.8546465757895638</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1"/>
       <c r="D29">
-        <v>159.2785172404551</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>164.01816820568561</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -829,7 +890,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -843,7 +904,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -851,13 +912,13 @@
         <v>44</v>
       </c>
       <c r="C35">
-        <v>1.966799645343378</v>
+        <v>1.973632985426387</v>
       </c>
       <c r="D35">
-        <v>1.888127659529643</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>1.8946876660093319</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -865,16 +926,16 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>0.4589199172467883</v>
+        <v>0.46051436326615708</v>
       </c>
       <c r="D36">
-        <v>0.4405631205569167</v>
+        <v>0.44209378873551092</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A24:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update LAOs data and move tests to package folder
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [target].xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [target].xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/LAOs/results/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_86F279D926C198CE8A160BD92BDEC1CF751C1DD1" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B923F291-EF47-4C68-BA14-BF35F5A11DB7}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Capital and operating costs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" iterateDelta="9.9999999999994451E-4"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
   <si>
     <t>Notes</t>
   </si>
@@ -103,34 +97,34 @@
     <t>Cost [MM$ / yr]</t>
   </si>
   <si>
+    <t>By-products and credits</t>
+  </si>
+  <si>
     <t>Raw materials</t>
   </si>
   <si>
-    <t>By-products and credits</t>
-  </si>
-  <si>
     <t>Total variable operating cost</t>
   </si>
   <si>
+    <t>Wastewater</t>
+  </si>
+  <si>
+    <t>Glucose</t>
+  </si>
+  <si>
+    <t>Process water</t>
+  </si>
+  <si>
+    <t>Tridecane</t>
+  </si>
+  <si>
+    <t>CSL</t>
+  </si>
+  <si>
     <t>DAP</t>
   </si>
   <si>
     <t>Salt</t>
-  </si>
-  <si>
-    <t>Wastewater</t>
-  </si>
-  <si>
-    <t>Glucose</t>
-  </si>
-  <si>
-    <t>Process water</t>
-  </si>
-  <si>
-    <t>Tridecane</t>
-  </si>
-  <si>
-    <t>CSL</t>
   </si>
   <si>
     <t>Natural gas</t>
@@ -160,8 +154,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,11 +207,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -227,14 +218,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -281,7 +264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -313,27 +296,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -365,24 +330,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -558,22 +505,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -581,7 +520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -589,10 +528,10 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>65.787766180879586</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>65.56319540899871</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -600,10 +539,10 @@
         <v>17</v>
       </c>
       <c r="C4">
-        <v>32.116801970507218</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32.40560529144166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -611,10 +550,10 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>2.6315106472351841</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2.622527816359948</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -622,10 +561,10 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>5.9208989562791627</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>5.900687586809884</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -633,10 +572,10 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>2.9604494781395809</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2.950343793404942</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -644,10 +583,10 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>109.4174272330407</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>109.4423598970151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -655,10 +594,10 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>10.94174272330407</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10.94423598970151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -666,10 +605,10 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>10.94174272330407</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10.94423598970151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -677,10 +616,10 @@
         <v>22</v>
       </c>
       <c r="C11">
-        <v>21.883485446608152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21.88847197940303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -688,10 +627,10 @@
         <v>23</v>
       </c>
       <c r="C12">
-        <v>32.825228169912222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>32.83270796910454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -699,10 +638,10 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>10.94174272330407</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>10.94423598970151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -710,10 +649,10 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>87.533941786432621</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>87.55388791761214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -721,10 +660,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>196.95136901947339</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>196.9962478146273</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -732,10 +671,10 @@
         <v>24</v>
       </c>
       <c r="C16">
-        <v>9.8475684509736681</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9.849812390731365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -743,10 +682,10 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>206.79893747044699</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>206.8460602053586</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
@@ -754,118 +693,116 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>30</v>
       </c>
       <c r="C21">
-        <v>895.39159499999994</v>
+        <v>-1.962995609856692</v>
       </c>
       <c r="D21">
-        <v>1.1811074895224249</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
+        <v>-6.266069596713132</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C22">
-        <v>136.07775000000001</v>
+        <v>240.404025</v>
       </c>
       <c r="D22">
-        <v>4.2304986641846387</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>144.7370872673688</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C23">
-        <v>-1.9630611699040379</v>
+        <v>0.320236305</v>
       </c>
       <c r="D23">
-        <v>-6.2658539245062812</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>27</v>
-      </c>
+        <v>0.9954177967561536</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C24">
-        <v>244.03276500000001</v>
+        <v>878.1550799999999</v>
       </c>
       <c r="D24">
-        <v>146.92179801857401</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="2"/>
+        <v>0.002402636063926985</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>0.320236305</v>
+        <v>51.528108</v>
       </c>
       <c r="D25">
-        <v>0.99534905024449527</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="2"/>
+        <v>0.5665456791641987</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C26">
-        <v>878.15507999999988</v>
+        <v>895.3915949999999</v>
       </c>
       <c r="D26">
-        <v>2.4024701315892168E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="2"/>
+        <v>1.181188778425073</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C27">
-        <v>51.528108000000003</v>
+        <v>136.07775</v>
       </c>
       <c r="D27">
-        <v>0.56651201273216611</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="2"/>
+        <v>4.230790853725686</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C28">
-        <v>197.76633000000001</v>
+        <v>197.76633</v>
       </c>
       <c r="D28">
-        <v>3.8546465757895638</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.954929396805927</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1"/>
       <c r="D29">
-        <v>164.01816820568561</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>161.934432005023</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -876,7 +813,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -890,7 +827,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -904,7 +841,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -912,13 +849,13 @@
         <v>44</v>
       </c>
       <c r="C35">
-        <v>1.973632985426387</v>
+        <v>1.966895862269961</v>
       </c>
       <c r="D35">
-        <v>1.8946876660093319</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1.888220027779163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -926,16 +863,15 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>0.46051436326615708</v>
+        <v>0.458942367862991</v>
       </c>
       <c r="D36">
-        <v>0.44209378873551092</v>
+        <v>0.4405846731484713</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A24:A28"/>
+  <mergeCells count="1">
+    <mergeCell ref="A22:A28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ad new biorefineries and update LAOs results
</commit_message>
<xml_diff>
--- a/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [target].xlsx
+++ b/BioSTEAM 2.x.x/biorefineries/LAOs/results/Capital and operating costs [target].xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/733a0933307f0df0/Code/Bioindustrial-Park/BioSTEAM 2.x.x/biorefineries/LAOs/results/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{6DC4926F-5118-4E91-B7D1-C178DF85EB27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="4044" yWindow="1932" windowWidth="17280" windowHeight="10044" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Capital and operating costs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -154,8 +160,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,8 +213,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -218,6 +227,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -264,7 +281,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -296,9 +313,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -330,6 +365,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -505,14 +558,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -520,7 +573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -528,10 +581,10 @@
         <v>17</v>
       </c>
       <c r="C3">
-        <v>65.56319540899871</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>65.563195408998709</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -542,7 +595,7 @@
         <v>32.40560529144166</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -550,10 +603,10 @@
         <v>18</v>
       </c>
       <c r="C5">
-        <v>2.622527816359948</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>2.6225278163599479</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -561,10 +614,10 @@
         <v>19</v>
       </c>
       <c r="C6">
-        <v>5.900687586809884</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>5.9006875868098838</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -572,10 +625,10 @@
         <v>20</v>
       </c>
       <c r="C7">
-        <v>2.950343793404942</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>2.9503437934049419</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -583,10 +636,10 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>109.4423598970151</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>109.44235989701509</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -594,10 +647,10 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <v>10.94423598970151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>10.944235989701509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -605,10 +658,10 @@
         <v>21</v>
       </c>
       <c r="C10">
-        <v>10.94423598970151</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>10.944235989701509</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -616,10 +669,10 @@
         <v>22</v>
       </c>
       <c r="C11">
-        <v>21.88847197940303</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>21.888471979403029</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -630,7 +683,7 @@
         <v>32.83270796910454</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -638,10 +691,10 @@
         <v>21</v>
       </c>
       <c r="C13">
-        <v>10.94423598970151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>10.944235989701509</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -649,10 +702,10 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <v>87.55388791761214</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
+        <v>87.553887917612144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -660,10 +713,10 @@
         <v>17</v>
       </c>
       <c r="C15">
-        <v>196.9962478146273</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
+        <v>196.99624781462731</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -671,10 +724,10 @@
         <v>24</v>
       </c>
       <c r="C16">
-        <v>9.849812390731365</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>9.8498123907313655</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -682,10 +735,10 @@
         <v>17</v>
       </c>
       <c r="C17">
-        <v>206.8460602053586</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>206.84606020535861</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
@@ -693,7 +746,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
@@ -701,28 +754,28 @@
         <v>30</v>
       </c>
       <c r="C21">
-        <v>-1.962995609856692</v>
+        <v>-1.9629956098566921</v>
       </c>
       <c r="D21">
-        <v>-6.266069596713132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
+        <v>-6.2660695967131321</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C22">
-        <v>240.404025</v>
+        <v>240.40402499999999</v>
       </c>
       <c r="D22">
-        <v>144.7370872673688</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1"/>
+        <v>144.73708726736879</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
@@ -730,79 +783,79 @@
         <v>0.320236305</v>
       </c>
       <c r="D23">
-        <v>0.9954177967561536</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1"/>
+        <v>0.99541779675615361</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="2"/>
       <c r="B24" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C24">
-        <v>878.1550799999999</v>
+        <v>878.15507999999988</v>
       </c>
       <c r="D24">
-        <v>0.002402636063926985</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1"/>
+        <v>2.4026360639269849E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="2"/>
       <c r="B25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C25">
-        <v>51.528108</v>
+        <v>51.528108000000003</v>
       </c>
       <c r="D25">
-        <v>0.5665456791641987</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1"/>
+        <v>0.56654567916419873</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="2"/>
       <c r="B26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C26">
-        <v>895.3915949999999</v>
+        <v>895.39159499999994</v>
       </c>
       <c r="D26">
         <v>1.181188778425073</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="2"/>
       <c r="B27" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C27">
-        <v>136.07775</v>
+        <v>136.07775000000001</v>
       </c>
       <c r="D27">
-        <v>4.230790853725686</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1"/>
+        <v>4.2307908537256864</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2"/>
       <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
       <c r="C28">
-        <v>197.76633</v>
+        <v>197.76633000000001</v>
       </c>
       <c r="D28">
-        <v>3.954929396805927</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>3.9549293968059271</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" s="1"/>
       <c r="D29">
-        <v>161.934432005023</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>161.93443200502301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,7 +866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>39</v>
       </c>
@@ -827,7 +880,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>40</v>
       </c>
@@ -841,7 +894,7 @@
         <v>2.16</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>41</v>
       </c>
@@ -855,7 +908,7 @@
         <v>1.888220027779163</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>42</v>
       </c>
@@ -863,10 +916,10 @@
         <v>44</v>
       </c>
       <c r="C36">
-        <v>0.458942367862991</v>
+        <v>0.45894236786299097</v>
       </c>
       <c r="D36">
-        <v>0.4405846731484713</v>
+        <v>0.44058467314847127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>